<commit_message>
Quick save before branch
</commit_message>
<xml_diff>
--- a/NamMatlab/QRL/MatlabImages/parameters.xlsx
+++ b/NamMatlab/QRL/MatlabImages/parameters.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="90" windowWidth="13395" windowHeight="9780" activeTab="3"/>
+    <workbookView xWindow="360" yWindow="90" windowWidth="13395" windowHeight="9780" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="54" sheetId="2" r:id="rId2"/>
     <sheet name="55" sheetId="3" r:id="rId3"/>
     <sheet name="56" sheetId="4" r:id="rId4"/>
+    <sheet name="57" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="25">
   <si>
     <t>filenumber</t>
   </si>
@@ -874,6 +875,221 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B25"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>4.34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>0.315</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>8.2000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>8.4500000000000006E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>0.13769999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>8.81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>52.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>0.97499999999999998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>0.97499999999999998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>0.98</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B25"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:B25"/>
     </sheetView>
@@ -885,7 +1101,7 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Changed lqr sim. Cleaned up runfile
</commit_message>
<xml_diff>
--- a/NamMatlab/QRL/MatlabImages/parameters.xlsx
+++ b/NamMatlab/QRL/MatlabImages/parameters.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="90" windowWidth="13395" windowHeight="9780"/>
+    <workbookView xWindow="360" yWindow="90" windowWidth="13395" windowHeight="9780" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -16,13 +16,14 @@
     <sheet name="61" sheetId="7" r:id="rId7"/>
     <sheet name="62" sheetId="8" r:id="rId8"/>
     <sheet name="63" sheetId="9" r:id="rId9"/>
+    <sheet name="64" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="34">
   <si>
     <t>filenumber</t>
   </si>
@@ -474,7 +475,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
@@ -496,27 +497,27 @@
         <v>9</v>
       </c>
       <c r="E2" s="1" t="str">
-        <f ca="1">INDIRECT("'"&amp;E$1&amp;"'!A"&amp;$D2)</f>
+        <f t="shared" ref="E2:E7" ca="1" si="0">INDIRECT("'"&amp;E$1&amp;"'!A"&amp;$D2)</f>
         <v>kR</v>
       </c>
       <c r="F2" s="1">
-        <f ca="1">INDIRECT("'"&amp;E$1&amp;"'!B"&amp;$D2)</f>
+        <f t="shared" ref="F2:F7" ca="1" si="1">INDIRECT("'"&amp;E$1&amp;"'!B"&amp;$D2)</f>
         <v>0.98100000000000009</v>
       </c>
       <c r="G2" s="1" t="str">
-        <f ca="1">INDIRECT("'"&amp;G$1&amp;"'!A"&amp;$D2)</f>
+        <f t="shared" ref="G2:G7" ca="1" si="2">INDIRECT("'"&amp;G$1&amp;"'!A"&amp;$D2)</f>
         <v>kR</v>
       </c>
       <c r="H2" s="1">
-        <f ca="1">INDIRECT("'"&amp;G$1&amp;"'!B"&amp;$D2)</f>
+        <f t="shared" ref="H2:H7" ca="1" si="3">INDIRECT("'"&amp;G$1&amp;"'!B"&amp;$D2)</f>
         <v>0.98100000000000009</v>
       </c>
       <c r="I2" s="1" t="e">
-        <f ca="1">INDIRECT("'"&amp;I$1&amp;"'!A"&amp;$D2)</f>
+        <f t="shared" ref="I2:I7" ca="1" si="4">INDIRECT("'"&amp;I$1&amp;"'!A"&amp;$D2)</f>
         <v>#REF!</v>
       </c>
       <c r="J2" s="1" t="e">
-        <f ca="1">INDIRECT("'"&amp;I$1&amp;"'!B"&amp;$D2)</f>
+        <f t="shared" ref="J2:J7" ca="1" si="5">INDIRECT("'"&amp;I$1&amp;"'!B"&amp;$D2)</f>
         <v>#REF!</v>
       </c>
     </row>
@@ -525,27 +526,27 @@
         <v>10</v>
       </c>
       <c r="E3" s="1" t="str">
-        <f ca="1">INDIRECT("'"&amp;E$1&amp;"'!A"&amp;$D3)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>kOmega</v>
       </c>
       <c r="F3" s="1">
-        <f ca="1">INDIRECT("'"&amp;E$1&amp;"'!B"&amp;$D3)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0.1</v>
       </c>
       <c r="G3" s="1" t="str">
-        <f ca="1">INDIRECT("'"&amp;G$1&amp;"'!A"&amp;$D3)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>kOmega</v>
       </c>
       <c r="H3" s="1">
-        <f ca="1">INDIRECT("'"&amp;G$1&amp;"'!B"&amp;$D3)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0.45</v>
       </c>
       <c r="I3" s="1" t="e">
-        <f ca="1">INDIRECT("'"&amp;I$1&amp;"'!A"&amp;$D3)</f>
+        <f t="shared" ca="1" si="4"/>
         <v>#REF!</v>
       </c>
       <c r="J3" s="1" t="e">
-        <f ca="1">INDIRECT("'"&amp;I$1&amp;"'!B"&amp;$D3)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>#REF!</v>
       </c>
     </row>
@@ -554,27 +555,27 @@
         <v>11</v>
       </c>
       <c r="E4" s="1" t="str">
-        <f ca="1">INDIRECT("'"&amp;E$1&amp;"'!A"&amp;$D4)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>kq</v>
       </c>
       <c r="F4" s="1">
-        <f ca="1">INDIRECT("'"&amp;E$1&amp;"'!B"&amp;$D4)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>10</v>
       </c>
       <c r="G4" s="1" t="str">
-        <f ca="1">INDIRECT("'"&amp;G$1&amp;"'!A"&amp;$D4)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>kq</v>
       </c>
       <c r="H4" s="1">
-        <f ca="1">INDIRECT("'"&amp;G$1&amp;"'!B"&amp;$D4)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>10</v>
       </c>
       <c r="I4" s="1" t="e">
-        <f ca="1">INDIRECT("'"&amp;I$1&amp;"'!A"&amp;$D4)</f>
+        <f t="shared" ca="1" si="4"/>
         <v>#REF!</v>
       </c>
       <c r="J4" s="1" t="e">
-        <f ca="1">INDIRECT("'"&amp;I$1&amp;"'!B"&amp;$D4)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>#REF!</v>
       </c>
     </row>
@@ -583,27 +584,27 @@
         <v>12</v>
       </c>
       <c r="E5" s="1" t="str">
-        <f ca="1">INDIRECT("'"&amp;E$1&amp;"'!A"&amp;$D5)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>komega</v>
       </c>
       <c r="F5" s="1">
-        <f ca="1">INDIRECT("'"&amp;E$1&amp;"'!B"&amp;$D5)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>7.5</v>
       </c>
       <c r="G5" s="1" t="str">
-        <f ca="1">INDIRECT("'"&amp;G$1&amp;"'!A"&amp;$D5)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>komega</v>
       </c>
       <c r="H5" s="1">
-        <f ca="1">INDIRECT("'"&amp;G$1&amp;"'!B"&amp;$D5)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>7.5</v>
       </c>
       <c r="I5" s="1" t="e">
-        <f ca="1">INDIRECT("'"&amp;I$1&amp;"'!A"&amp;$D5)</f>
+        <f t="shared" ca="1" si="4"/>
         <v>#REF!</v>
       </c>
       <c r="J5" s="1" t="e">
-        <f ca="1">INDIRECT("'"&amp;I$1&amp;"'!B"&amp;$D5)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>#REF!</v>
       </c>
     </row>
@@ -612,27 +613,27 @@
         <v>13</v>
       </c>
       <c r="E6" s="1" t="str">
-        <f ca="1">INDIRECT("'"&amp;E$1&amp;"'!A"&amp;$D6)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>kpx</v>
       </c>
       <c r="F6" s="1">
-        <f ca="1">INDIRECT("'"&amp;E$1&amp;"'!B"&amp;$D6)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>10</v>
       </c>
       <c r="G6" s="1" t="str">
-        <f ca="1">INDIRECT("'"&amp;G$1&amp;"'!A"&amp;$D6)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>kpx</v>
       </c>
       <c r="H6" s="1">
-        <f ca="1">INDIRECT("'"&amp;G$1&amp;"'!B"&amp;$D6)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>10</v>
       </c>
       <c r="I6" s="1" t="e">
-        <f ca="1">INDIRECT("'"&amp;I$1&amp;"'!A"&amp;$D6)</f>
+        <f t="shared" ca="1" si="4"/>
         <v>#REF!</v>
       </c>
       <c r="J6" s="1" t="e">
-        <f ca="1">INDIRECT("'"&amp;I$1&amp;"'!B"&amp;$D6)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>#REF!</v>
       </c>
     </row>
@@ -641,27 +642,27 @@
         <v>14</v>
       </c>
       <c r="E7" s="1" t="str">
-        <f ca="1">INDIRECT("'"&amp;E$1&amp;"'!A"&amp;$D7)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>kdx</v>
       </c>
       <c r="F7" s="1">
-        <f ca="1">INDIRECT("'"&amp;E$1&amp;"'!B"&amp;$D7)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>3</v>
       </c>
       <c r="G7" s="1" t="str">
-        <f ca="1">INDIRECT("'"&amp;G$1&amp;"'!A"&amp;$D7)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>kdx</v>
       </c>
       <c r="H7" s="1">
-        <f ca="1">INDIRECT("'"&amp;G$1&amp;"'!B"&amp;$D7)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>3</v>
       </c>
       <c r="I7" s="1" t="e">
-        <f ca="1">INDIRECT("'"&amp;I$1&amp;"'!A"&amp;$D7)</f>
+        <f t="shared" ca="1" si="4"/>
         <v>#REF!</v>
       </c>
       <c r="J7" s="1" t="e">
-        <f ca="1">INDIRECT("'"&amp;I$1&amp;"'!B"&amp;$D7)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>#REF!</v>
       </c>
     </row>
@@ -679,21 +680,21 @@
         <v>26</v>
       </c>
       <c r="E9">
-        <f ca="1">F2</f>
+        <f t="shared" ref="E9:E14" ca="1" si="6">F2</f>
         <v>0.98100000000000009</v>
       </c>
       <c r="F9" t="s">
         <v>26</v>
       </c>
       <c r="G9">
-        <f ca="1">H2</f>
+        <f t="shared" ref="G9:G14" ca="1" si="7">H2</f>
         <v>0.98100000000000009</v>
       </c>
       <c r="H9" t="s">
         <v>26</v>
       </c>
       <c r="I9" t="e">
-        <f ca="1">J2</f>
+        <f t="shared" ref="I9:I14" ca="1" si="8">J2</f>
         <v>#REF!</v>
       </c>
       <c r="J9" s="2" t="s">
@@ -714,21 +715,21 @@
         <v>26</v>
       </c>
       <c r="E10">
-        <f ca="1">F3</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0.1</v>
       </c>
       <c r="F10" t="s">
         <v>26</v>
       </c>
       <c r="G10">
-        <f ca="1">H3</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0.45</v>
       </c>
       <c r="H10" t="s">
         <v>26</v>
       </c>
       <c r="I10" t="e">
-        <f ca="1">J3</f>
+        <f t="shared" ca="1" si="8"/>
         <v>#REF!</v>
       </c>
       <c r="J10" s="2" t="s">
@@ -749,21 +750,21 @@
         <v>26</v>
       </c>
       <c r="E11">
-        <f ca="1">F4</f>
+        <f t="shared" ca="1" si="6"/>
         <v>10</v>
       </c>
       <c r="F11" t="s">
         <v>26</v>
       </c>
       <c r="G11">
-        <f ca="1">H4</f>
+        <f t="shared" ca="1" si="7"/>
         <v>10</v>
       </c>
       <c r="H11" t="s">
         <v>26</v>
       </c>
       <c r="I11" t="e">
-        <f ca="1">J4</f>
+        <f t="shared" ca="1" si="8"/>
         <v>#REF!</v>
       </c>
       <c r="J11" s="2" t="s">
@@ -784,21 +785,21 @@
         <v>26</v>
       </c>
       <c r="E12">
-        <f ca="1">F5</f>
+        <f t="shared" ca="1" si="6"/>
         <v>7.5</v>
       </c>
       <c r="F12" t="s">
         <v>26</v>
       </c>
       <c r="G12">
-        <f ca="1">H5</f>
+        <f t="shared" ca="1" si="7"/>
         <v>7.5</v>
       </c>
       <c r="H12" t="s">
         <v>26</v>
       </c>
       <c r="I12" t="e">
-        <f ca="1">J5</f>
+        <f t="shared" ca="1" si="8"/>
         <v>#REF!</v>
       </c>
       <c r="J12" s="2" t="s">
@@ -819,21 +820,21 @@
         <v>26</v>
       </c>
       <c r="E13">
-        <f ca="1">F6</f>
+        <f t="shared" ca="1" si="6"/>
         <v>10</v>
       </c>
       <c r="F13" t="s">
         <v>26</v>
       </c>
       <c r="G13">
-        <f ca="1">H6</f>
+        <f t="shared" ca="1" si="7"/>
         <v>10</v>
       </c>
       <c r="H13" t="s">
         <v>26</v>
       </c>
       <c r="I13" t="e">
-        <f ca="1">J6</f>
+        <f t="shared" ca="1" si="8"/>
         <v>#REF!</v>
       </c>
       <c r="J13" s="2" t="s">
@@ -854,21 +855,21 @@
         <v>26</v>
       </c>
       <c r="E14">
-        <f ca="1">F7</f>
+        <f t="shared" ca="1" si="6"/>
         <v>3</v>
       </c>
       <c r="F14" t="s">
         <v>26</v>
       </c>
       <c r="G14">
-        <f ca="1">H7</f>
+        <f t="shared" ca="1" si="7"/>
         <v>3</v>
       </c>
       <c r="H14" t="s">
         <v>26</v>
       </c>
       <c r="I14" t="e">
-        <f ca="1">J7</f>
+        <f t="shared" ca="1" si="8"/>
         <v>#REF!</v>
       </c>
       <c r="J14" s="2" t="s">
@@ -878,6 +879,221 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>0.126</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>2.2300000000000002E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>2.99E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>4.7999999999999996E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>0.98100000000000009</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>0.98</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>